<commit_message>
update new files and model cleaning
</commit_message>
<xml_diff>
--- a/Data/fur_dataset_clean.xlsx
+++ b/Data/fur_dataset_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myjcuedu-my.sharepoint.com/personal/alejandro_delafuentepinero1_my_jcu_edu_au/Documents/PhD - projects/Ringtail - Mechanistic model - Wet Tropics/Ringtail_WT_Mechanistic_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="8_{74CE4A96-530B-7F45-AF16-549FE02BD4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AA6D2C6-E8A1-6F41-9FAD-E7ABAC3BD65C}"/>
+  <xr:revisionPtr revIDLastSave="473" documentId="8_{74CE4A96-530B-7F45-AF16-549FE02BD4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{798E5012-580E-774A-BD99-17DB77433F0D}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="860" windowWidth="16980" windowHeight="20120" xr2:uid="{FFA2A11C-E7F5-B849-9C8E-0C9A229E8402}"/>
+    <workbookView xWindow="120" yWindow="860" windowWidth="16980" windowHeight="20120" xr2:uid="{FFA2A11C-E7F5-B849-9C8E-0C9A229E8402}"/>
   </bookViews>
   <sheets>
     <sheet name="fur_dataset" sheetId="1" r:id="rId1"/>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C267A2-F2D1-FA4E-858E-641C66C9A0B3}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,7 +1240,7 @@
         <v>18</v>
       </c>
       <c r="F15">
-        <v>84828636.64721866</v>
+        <v>84828636.647218704</v>
       </c>
       <c r="G15">
         <v>38580649.332079038</v>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="F17">
         <f>SUM(F15:F16)</f>
-        <v>85992877.894101426</v>
+        <v>85992877.894101471</v>
       </c>
       <c r="I17">
         <v>7</v>

</xml_diff>